<commit_message>
Double-notched rotors + active lamp panel
Double-notched rotors logic has been implemented.  The output lamp panel is now active and presenting current letter being enciphered.
</commit_message>
<xml_diff>
--- a/Schemat połączeń.xlsx
+++ b/Schemat połączeń.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="22995" windowHeight="10050"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="21690" windowHeight="10050"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -247,12 +247,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -556,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AL30" sqref="AL30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2696,7 +2697,7 @@
       <c r="AB16">
         <v>23</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AD16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="AE16">
@@ -2711,7 +2712,7 @@
       <c r="AI16">
         <v>18</v>
       </c>
-      <c r="AK16" t="s">
+      <c r="AK16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="AL16">
@@ -2726,7 +2727,7 @@
       <c r="AP16">
         <v>6</v>
       </c>
-      <c r="AR16" t="s">
+      <c r="AR16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="AS16">
@@ -2741,7 +2742,7 @@
       <c r="AW16">
         <v>8</v>
       </c>
-      <c r="AY16" t="s">
+      <c r="AY16" s="3" t="s">
         <v>12</v>
       </c>
       <c r="AZ16">
@@ -4687,7 +4688,7 @@
       <c r="AI29">
         <v>1</v>
       </c>
-      <c r="AK29" t="s">
+      <c r="AK29" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AL29">
@@ -4702,7 +4703,7 @@
       <c r="AP29">
         <v>14</v>
       </c>
-      <c r="AR29" t="s">
+      <c r="AR29" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AS29">
@@ -4717,7 +4718,7 @@
       <c r="AW29">
         <v>1</v>
       </c>
-      <c r="AY29" t="s">
+      <c r="AY29" s="3" t="s">
         <v>25</v>
       </c>
       <c r="AZ29">
@@ -4761,6 +4762,12 @@
       </c>
       <c r="BR29">
         <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:70" x14ac:dyDescent="0.25">
+      <c r="AL30">
+        <f>AL29-AL16</f>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="2:35" ht="18.75" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Stepping logic debugged and finally well designed
The stepping mechanism has been implemented fainally in a propper way. Various visual widgets and tweak have been done.
</commit_message>
<xml_diff>
--- a/Schemat połączeń.xlsx
+++ b/Schemat połączeń.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="46">
   <si>
     <t>A</t>
   </si>
@@ -557,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:BR62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AL30" sqref="AL30"/>
+    <sheetView tabSelected="1" topLeftCell="V37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB51" sqref="AB51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4770,7 +4770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="2:35" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:34" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
@@ -4787,7 +4787,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>26</v>
       </c>
@@ -4824,20 +4824,14 @@
       <c r="X35" t="s">
         <v>27</v>
       </c>
-      <c r="AA35" t="s">
-        <v>28</v>
-      </c>
       <c r="AD35" t="s">
         <v>26</v>
       </c>
       <c r="AE35" t="s">
         <v>27</v>
       </c>
-      <c r="AH35" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>30</v>
       </c>
@@ -4880,26 +4874,14 @@
       <c r="Y36" t="s">
         <v>31</v>
       </c>
-      <c r="AA36" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>31</v>
-      </c>
       <c r="AE36" t="s">
         <v>30</v>
       </c>
       <c r="AF36" t="s">
         <v>31</v>
       </c>
-      <c r="AH36" t="s">
-        <v>30</v>
-      </c>
-      <c r="AI36" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>0</v>
       </c>
@@ -4951,7 +4933,9 @@
       <c r="X37">
         <v>0</v>
       </c>
-      <c r="Y37" s="2"/>
+      <c r="Y37" s="2">
+        <v>4</v>
+      </c>
       <c r="AA37" s="2"/>
       <c r="AD37" t="s">
         <v>0</v>
@@ -4959,10 +4943,12 @@
       <c r="AE37">
         <v>0</v>
       </c>
-      <c r="AF37" s="2"/>
+      <c r="AF37" s="2">
+        <v>17</v>
+      </c>
       <c r="AH37" s="2"/>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>1</v>
       </c>
@@ -5014,7 +5000,9 @@
       <c r="X38">
         <v>1</v>
       </c>
-      <c r="Y38" s="2"/>
+      <c r="Y38" s="2">
+        <v>13</v>
+      </c>
       <c r="AA38" s="2"/>
       <c r="AD38" t="s">
         <v>1</v>
@@ -5022,10 +5010,12 @@
       <c r="AE38">
         <v>1</v>
       </c>
-      <c r="AF38" s="2"/>
+      <c r="AF38" s="2">
+        <v>3</v>
+      </c>
       <c r="AH38" s="2"/>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>2</v>
       </c>
@@ -5077,7 +5067,9 @@
       <c r="X39">
         <v>2</v>
       </c>
-      <c r="Y39" s="2"/>
+      <c r="Y39" s="2">
+        <v>10</v>
+      </c>
       <c r="AA39" s="2"/>
       <c r="AD39" t="s">
         <v>2</v>
@@ -5085,10 +5077,12 @@
       <c r="AE39">
         <v>2</v>
       </c>
-      <c r="AF39" s="2"/>
+      <c r="AF39" s="2">
+        <v>14</v>
+      </c>
       <c r="AH39" s="2"/>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -5140,7 +5134,9 @@
       <c r="X40">
         <v>3</v>
       </c>
-      <c r="Y40" s="2"/>
+      <c r="Y40" s="2">
+        <v>16</v>
+      </c>
       <c r="AA40" s="2"/>
       <c r="AD40" t="s">
         <v>3</v>
@@ -5148,10 +5144,12 @@
       <c r="AE40">
         <v>3</v>
       </c>
-      <c r="AF40" s="2"/>
+      <c r="AF40" s="2">
+        <v>1</v>
+      </c>
       <c r="AH40" s="2"/>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>4</v>
       </c>
@@ -5203,7 +5201,9 @@
       <c r="X41">
         <v>4</v>
       </c>
-      <c r="Y41" s="2"/>
+      <c r="Y41" s="2">
+        <v>0</v>
+      </c>
       <c r="AA41" s="2"/>
       <c r="AD41" t="s">
         <v>4</v>
@@ -5211,10 +5211,12 @@
       <c r="AE41">
         <v>4</v>
       </c>
-      <c r="AF41" s="2"/>
+      <c r="AF41" s="2">
+        <v>9</v>
+      </c>
       <c r="AH41" s="2"/>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>5</v>
       </c>
@@ -5266,7 +5268,9 @@
       <c r="X42">
         <v>5</v>
       </c>
-      <c r="Y42" s="2"/>
+      <c r="Y42" s="2">
+        <v>20</v>
+      </c>
       <c r="AA42" s="2"/>
       <c r="AD42" t="s">
         <v>5</v>
@@ -5274,10 +5278,12 @@
       <c r="AE42">
         <v>5</v>
       </c>
-      <c r="AF42" s="2"/>
+      <c r="AF42" s="2">
+        <v>13</v>
+      </c>
       <c r="AH42" s="2"/>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>6</v>
       </c>
@@ -5329,7 +5335,9 @@
       <c r="X43">
         <v>6</v>
       </c>
-      <c r="Y43" s="2"/>
+      <c r="Y43" s="2">
+        <v>24</v>
+      </c>
       <c r="AA43" s="2"/>
       <c r="AD43" t="s">
         <v>6</v>
@@ -5337,10 +5345,12 @@
       <c r="AE43">
         <v>6</v>
       </c>
-      <c r="AF43" s="2"/>
+      <c r="AF43" s="2">
+        <v>19</v>
+      </c>
       <c r="AH43" s="2"/>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>7</v>
       </c>
@@ -5392,7 +5402,9 @@
       <c r="X44">
         <v>7</v>
       </c>
-      <c r="Y44" s="2"/>
+      <c r="Y44" s="2">
+        <v>22</v>
+      </c>
       <c r="AA44" s="2"/>
       <c r="AD44" t="s">
         <v>7</v>
@@ -5400,10 +5412,12 @@
       <c r="AE44">
         <v>7</v>
       </c>
-      <c r="AF44" s="2"/>
+      <c r="AF44" s="2">
+        <v>10</v>
+      </c>
       <c r="AH44" s="2"/>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>8</v>
       </c>
@@ -5455,7 +5469,9 @@
       <c r="X45">
         <v>8</v>
       </c>
-      <c r="Y45" s="2"/>
+      <c r="Y45" s="2">
+        <v>9</v>
+      </c>
       <c r="AA45" s="2"/>
       <c r="AD45" t="s">
         <v>8</v>
@@ -5463,10 +5479,12 @@
       <c r="AE45">
         <v>8</v>
       </c>
-      <c r="AF45" s="2"/>
+      <c r="AF45" s="2">
+        <v>21</v>
+      </c>
       <c r="AH45" s="2"/>
     </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>9</v>
       </c>
@@ -5518,7 +5536,9 @@
       <c r="X46">
         <v>9</v>
       </c>
-      <c r="Y46" s="2"/>
+      <c r="Y46" s="2">
+        <v>8</v>
+      </c>
       <c r="AA46" s="2"/>
       <c r="AD46" t="s">
         <v>9</v>
@@ -5526,10 +5546,12 @@
       <c r="AE46">
         <v>9</v>
       </c>
-      <c r="AF46" s="2"/>
+      <c r="AF46" s="2">
+        <v>4</v>
+      </c>
       <c r="AH46" s="2"/>
     </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>10</v>
       </c>
@@ -5581,7 +5603,9 @@
       <c r="X47">
         <v>10</v>
       </c>
-      <c r="Y47" s="2"/>
+      <c r="Y47" s="2">
+        <v>2</v>
+      </c>
       <c r="AA47" s="2"/>
       <c r="AD47" t="s">
         <v>10</v>
@@ -5589,10 +5613,12 @@
       <c r="AE47">
         <v>10</v>
       </c>
-      <c r="AF47" s="2"/>
+      <c r="AF47" s="2">
+        <v>7</v>
+      </c>
       <c r="AH47" s="2"/>
     </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>11</v>
       </c>
@@ -5644,7 +5670,9 @@
       <c r="X48">
         <v>11</v>
       </c>
-      <c r="Y48" s="2"/>
+      <c r="Y48" s="2">
+        <v>14</v>
+      </c>
       <c r="AA48" s="2"/>
       <c r="AD48" t="s">
         <v>11</v>
@@ -5652,7 +5680,9 @@
       <c r="AE48">
         <v>11</v>
       </c>
-      <c r="AF48" s="2"/>
+      <c r="AF48" s="2">
+        <v>12</v>
+      </c>
       <c r="AH48" s="2"/>
     </row>
     <row r="49" spans="2:34" x14ac:dyDescent="0.25">
@@ -5707,7 +5737,9 @@
       <c r="X49">
         <v>12</v>
       </c>
-      <c r="Y49" s="2"/>
+      <c r="Y49" s="2">
+        <v>15</v>
+      </c>
       <c r="AA49" s="2"/>
       <c r="AD49" t="s">
         <v>12</v>
@@ -5715,7 +5747,9 @@
       <c r="AE49">
         <v>12</v>
       </c>
-      <c r="AF49" s="2"/>
+      <c r="AF49" s="2">
+        <v>11</v>
+      </c>
       <c r="AH49" s="2"/>
     </row>
     <row r="50" spans="2:34" x14ac:dyDescent="0.25">
@@ -5770,7 +5804,9 @@
       <c r="X50">
         <v>13</v>
       </c>
-      <c r="Y50" s="2"/>
+      <c r="Y50" s="2">
+        <v>1</v>
+      </c>
       <c r="AA50" s="2"/>
       <c r="AD50" t="s">
         <v>13</v>
@@ -5778,7 +5814,9 @@
       <c r="AE50">
         <v>13</v>
       </c>
-      <c r="AF50" s="2"/>
+      <c r="AF50" s="2">
+        <v>5</v>
+      </c>
       <c r="AH50" s="2"/>
     </row>
     <row r="51" spans="2:34" x14ac:dyDescent="0.25">
@@ -5833,7 +5871,9 @@
       <c r="X51">
         <v>14</v>
       </c>
-      <c r="Y51" s="2"/>
+      <c r="Y51" s="2">
+        <v>11</v>
+      </c>
       <c r="AA51" s="2"/>
       <c r="AD51" t="s">
         <v>14</v>
@@ -5841,7 +5881,9 @@
       <c r="AE51">
         <v>14</v>
       </c>
-      <c r="AF51" s="2"/>
+      <c r="AF51" s="2">
+        <v>2</v>
+      </c>
       <c r="AH51" s="2"/>
     </row>
     <row r="52" spans="2:34" x14ac:dyDescent="0.25">
@@ -5896,7 +5938,9 @@
       <c r="X52">
         <v>15</v>
       </c>
-      <c r="Y52" s="2"/>
+      <c r="Y52" s="2">
+        <v>12</v>
+      </c>
       <c r="AA52" s="2"/>
       <c r="AD52" t="s">
         <v>15</v>
@@ -5904,7 +5948,9 @@
       <c r="AE52">
         <v>15</v>
       </c>
-      <c r="AF52" s="2"/>
+      <c r="AF52" s="2">
+        <v>22</v>
+      </c>
       <c r="AH52" s="2"/>
     </row>
     <row r="53" spans="2:34" x14ac:dyDescent="0.25">
@@ -5959,7 +6005,9 @@
       <c r="X53">
         <v>16</v>
       </c>
-      <c r="Y53" s="2"/>
+      <c r="Y53" s="2">
+        <v>3</v>
+      </c>
       <c r="AA53" s="2"/>
       <c r="AD53" t="s">
         <v>16</v>
@@ -5967,7 +6015,9 @@
       <c r="AE53">
         <v>16</v>
       </c>
-      <c r="AF53" s="2"/>
+      <c r="AF53" s="2">
+        <v>25</v>
+      </c>
       <c r="AH53" s="2"/>
     </row>
     <row r="54" spans="2:34" x14ac:dyDescent="0.25">
@@ -6022,7 +6072,9 @@
       <c r="X54">
         <v>17</v>
       </c>
-      <c r="Y54" s="2"/>
+      <c r="Y54" s="2">
+        <v>23</v>
+      </c>
       <c r="AA54" s="2"/>
       <c r="AD54" t="s">
         <v>17</v>
@@ -6030,7 +6082,9 @@
       <c r="AE54">
         <v>17</v>
       </c>
-      <c r="AF54" s="2"/>
+      <c r="AF54" s="2">
+        <v>0</v>
+      </c>
       <c r="AH54" s="2"/>
     </row>
     <row r="55" spans="2:34" x14ac:dyDescent="0.25">
@@ -6085,7 +6139,9 @@
       <c r="X55">
         <v>18</v>
       </c>
-      <c r="Y55" s="2"/>
+      <c r="Y55" s="2">
+        <v>25</v>
+      </c>
       <c r="AA55" s="2"/>
       <c r="AD55" t="s">
         <v>18</v>
@@ -6093,7 +6149,9 @@
       <c r="AE55">
         <v>18</v>
       </c>
-      <c r="AF55" s="2"/>
+      <c r="AF55" s="2">
+        <v>23</v>
+      </c>
       <c r="AH55" s="2"/>
     </row>
     <row r="56" spans="2:34" x14ac:dyDescent="0.25">
@@ -6148,7 +6206,9 @@
       <c r="X56">
         <v>19</v>
       </c>
-      <c r="Y56" s="2"/>
+      <c r="Y56" s="2">
+        <v>21</v>
+      </c>
       <c r="AA56" s="2"/>
       <c r="AD56" t="s">
         <v>19</v>
@@ -6156,7 +6216,9 @@
       <c r="AE56">
         <v>19</v>
       </c>
-      <c r="AF56" s="2"/>
+      <c r="AF56" s="2">
+        <v>6</v>
+      </c>
       <c r="AH56" s="2"/>
     </row>
     <row r="57" spans="2:34" x14ac:dyDescent="0.25">
@@ -6211,7 +6273,9 @@
       <c r="X57">
         <v>20</v>
       </c>
-      <c r="Y57" s="2"/>
+      <c r="Y57" s="2">
+        <v>5</v>
+      </c>
       <c r="AA57" s="2"/>
       <c r="AD57" t="s">
         <v>20</v>
@@ -6219,7 +6283,9 @@
       <c r="AE57">
         <v>20</v>
       </c>
-      <c r="AF57" s="2"/>
+      <c r="AF57" s="2">
+        <v>24</v>
+      </c>
       <c r="AH57" s="2"/>
     </row>
     <row r="58" spans="2:34" x14ac:dyDescent="0.25">
@@ -6274,7 +6340,9 @@
       <c r="X58">
         <v>21</v>
       </c>
-      <c r="Y58" s="2"/>
+      <c r="Y58" s="2">
+        <v>19</v>
+      </c>
       <c r="AA58" s="2"/>
       <c r="AD58" t="s">
         <v>22</v>
@@ -6282,7 +6350,9 @@
       <c r="AE58">
         <v>21</v>
       </c>
-      <c r="AF58" s="2"/>
+      <c r="AF58" s="2">
+        <v>8</v>
+      </c>
       <c r="AH58" s="2"/>
     </row>
     <row r="59" spans="2:34" x14ac:dyDescent="0.25">
@@ -6337,7 +6407,9 @@
       <c r="X59">
         <v>22</v>
       </c>
-      <c r="Y59" s="2"/>
+      <c r="Y59" s="2">
+        <v>7</v>
+      </c>
       <c r="AA59" s="2"/>
       <c r="AD59" t="s">
         <v>21</v>
@@ -6345,7 +6417,9 @@
       <c r="AE59">
         <v>22</v>
       </c>
-      <c r="AF59" s="2"/>
+      <c r="AF59" s="2">
+        <v>15</v>
+      </c>
       <c r="AH59" s="2"/>
     </row>
     <row r="60" spans="2:34" x14ac:dyDescent="0.25">
@@ -6400,7 +6474,9 @@
       <c r="X60">
         <v>23</v>
       </c>
-      <c r="Y60" s="2"/>
+      <c r="Y60" s="2">
+        <v>17</v>
+      </c>
       <c r="AA60" s="2"/>
       <c r="AD60" t="s">
         <v>23</v>
@@ -6408,7 +6484,9 @@
       <c r="AE60">
         <v>23</v>
       </c>
-      <c r="AF60" s="2"/>
+      <c r="AF60" s="2">
+        <v>18</v>
+      </c>
       <c r="AH60" s="2"/>
     </row>
     <row r="61" spans="2:34" x14ac:dyDescent="0.25">
@@ -6463,7 +6541,9 @@
       <c r="X61">
         <v>24</v>
       </c>
-      <c r="Y61" s="2"/>
+      <c r="Y61" s="2">
+        <v>6</v>
+      </c>
       <c r="AA61" s="2"/>
       <c r="AD61" t="s">
         <v>24</v>
@@ -6471,7 +6551,9 @@
       <c r="AE61">
         <v>24</v>
       </c>
-      <c r="AF61" s="2"/>
+      <c r="AF61" s="2">
+        <v>20</v>
+      </c>
       <c r="AH61" s="2"/>
     </row>
     <row r="62" spans="2:34" x14ac:dyDescent="0.25">
@@ -6526,7 +6608,9 @@
       <c r="X62">
         <v>25</v>
       </c>
-      <c r="Y62" s="2"/>
+      <c r="Y62" s="2">
+        <v>18</v>
+      </c>
       <c r="AA62" s="2"/>
       <c r="AD62" t="s">
         <v>25</v>
@@ -6534,7 +6618,9 @@
       <c r="AE62">
         <v>25</v>
       </c>
-      <c r="AF62" s="2"/>
+      <c r="AF62" s="2">
+        <v>16</v>
+      </c>
       <c r="AH62" s="2"/>
     </row>
   </sheetData>

</xml_diff>